<commit_message>
add stock to row report box movements
</commit_message>
<xml_diff>
--- a/api/utils/templates/xlsx/baseProductBoxMovement.xlsx
+++ b/api/utils/templates/xlsx/baseProductBoxMovement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugo\Desktop\Proyectos\MaxImport\resources\dev\max-import-backend\api\utils\templates\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugod\Desktop\proyectos\maximport\sources\max-import-backend\api\utils\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1302CEFE-FCAF-46BA-B102-2E7AC892C44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107F697B-7045-44E0-A0EC-331AB8401FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3F90E08B-5E6B-4E95-9F51-698F115049C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3F90E08B-5E6B-4E95-9F51-698F115049C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">CODIGO DE CAJA </t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>LISTA DE MOVIMIENTO DE CAJAS</t>
+  </si>
+  <si>
+    <t>STOCK</t>
   </si>
 </sst>
 </file>
@@ -119,9 +122,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -143,7 +149,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -439,75 +445,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF94AF20-A2FF-4736-94BE-B00DDB288A13}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
fix: update relation stock value
</commit_message>
<xml_diff>
--- a/api/utils/templates/xlsx/baseProductBoxMovement.xlsx
+++ b/api/utils/templates/xlsx/baseProductBoxMovement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hugod\Desktop\proyectos\maximport\sources\max-import-backend\api\utils\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107F697B-7045-44E0-A0EC-331AB8401FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4D35E5-3CED-47CE-957F-33D4C237325F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3F90E08B-5E6B-4E95-9F51-698F115049C6}"/>
   </bookViews>
@@ -122,13 +122,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -448,13 +451,13 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="16" style="4" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>

</xml_diff>